<commit_message>
Add new disease files and update ExportResourceMappingConfig - Neuro Diseases
</commit_message>
<xml_diff>
--- a/src/main/groovy/projects/gecco/crf/GroovyGeneratorFromTemplate/values_NeuroDiseases.xlsx
+++ b/src/main/groovy/projects/gecco/crf/GroovyGeneratorFromTemplate/values_NeuroDiseases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario Macedo\PycharmProjects\ngu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario Macedo\IdeaProjects\kairos-fhir-dsl-mapping-example\src\main\groovy\projects\gecco\crf\GroovyGeneratorFromTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C70C096-E5DB-4274-8C51-4024932ABE5E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA7091C-CABF-4D5A-ACEC-0588102A1861}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
   <si>
     <t>Chronische neurologische Erkrankung</t>
   </si>
@@ -88,9 +88,6 @@
     <t>COV_GECCO_NEURO_ERKRANKUNG_MULTIPLE_SKLEROSE</t>
   </si>
   <si>
-    <t>Neuromuskuläre Erkrankungen</t>
-  </si>
-  <si>
     <t>COV_GECCO_NEURO_ERKRANKUNG_NEUROMUSKULÄRE_ERKRANKUNGEN</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t>Leidet der/die Patient*in an Epilepsie?</t>
   </si>
   <si>
-    <t>Migräne</t>
-  </si>
-  <si>
     <t>COV_GECCO_NEURO_ERKRANKUNG_MIGRÄNE</t>
   </si>
   <si>
@@ -214,9 +208,6 @@
     <t>MultipleSklerose</t>
   </si>
   <si>
-    <t>NeuromuskuläreErkrankungen</t>
-  </si>
-  <si>
     <t>Migraene</t>
   </si>
   <si>
@@ -257,6 +248,12 @@
   </si>
   <si>
     <t>G43.9</t>
+  </si>
+  <si>
+    <t>Neuromuskulaere Erkrankungen</t>
+  </si>
+  <si>
+    <t>NeuromuskulaereErkrankungen</t>
   </si>
 </sst>
 </file>
@@ -1617,7 +1614,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1638,25 +1635,25 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="F1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>58</v>
       </c>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
@@ -1664,16 +1661,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E2" s="11">
         <v>128283000</v>
@@ -1691,16 +1688,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E3" s="11">
         <v>74732009</v>
@@ -1709,7 +1706,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
@@ -1721,13 +1718,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E4" s="11">
         <v>197480006</v>
@@ -1748,13 +1745,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E5" s="11">
         <v>35489007</v>
@@ -1763,7 +1760,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
@@ -1775,13 +1772,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E6" s="11">
         <v>69322001</v>
@@ -1799,16 +1796,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E7" s="11">
         <v>49049000</v>
@@ -1829,13 +1826,13 @@
         <v>16</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E8" s="11">
         <v>52448006</v>
@@ -1853,16 +1850,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E9" s="11">
         <v>24700007</v>
@@ -1871,7 +1868,7 @@
         <v>20</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
@@ -1880,25 +1877,25 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E10" s="11">
         <v>257277002</v>
       </c>
       <c r="F10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>23</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -1907,25 +1904,25 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E11" s="11">
         <v>84757009</v>
       </c>
       <c r="F11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>25</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>26</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
@@ -1934,25 +1931,25 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E12" s="11">
         <v>37796009</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -1961,23 +1958,23 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11">
         <v>440140008</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -1986,23 +1983,23 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11">
         <v>429993008</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>

</xml_diff>